<commit_message>
Update test-results.xlsx file for admin features
</commit_message>
<xml_diff>
--- a/Testing/test-results.xlsx
+++ b/Testing/test-results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c71f1b740f59de2e/Documentos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mathiascagnoni/Desktop/Spoty List/TESTING/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="225" documentId="8_{359D4ED0-668A-1846-9DB3-0C434C6C9F2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84DCB9BB-78A5-9941-89D0-F33DF7E62F0B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C4DECF-D32E-A64E-A31C-238F2D1BC186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8320" yWindow="500" windowWidth="40560" windowHeight="28300" xr2:uid="{5DD9BFE7-A81A-D045-A251-B84427BB3CFB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="208">
   <si>
     <t>Test Execution Report</t>
   </si>
@@ -660,6 +660,9 @@
   </si>
   <si>
     <t>If you are signed in, click theLogout button</t>
+  </si>
+  <si>
+    <t>Log in with username admin and password admin</t>
   </si>
 </sst>
 </file>
@@ -1010,22 +1013,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
@@ -1349,8 +1352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5BC6B51-70E6-7143-A566-3069D36F620C}">
   <dimension ref="A1:K123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42"/>
+    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D107" sqref="D107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1367,16 +1370,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="27" thickBot="1">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
     </row>
     <row r="2" spans="1:8" ht="18" thickTop="1">
       <c r="A2" s="2" t="s">
@@ -1405,7 +1408,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="34">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="28" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="10" t="s">
@@ -1429,7 +1432,7 @@
       <c r="H3" s="14"/>
     </row>
     <row r="4" spans="1:8" ht="68">
-      <c r="A4" s="30"/>
+      <c r="A4" s="29"/>
       <c r="B4" s="5"/>
       <c r="C4" s="8">
         <v>2</v>
@@ -1449,7 +1452,7 @@
       <c r="H4" s="14"/>
     </row>
     <row r="5" spans="1:8" ht="68">
-      <c r="A5" s="30"/>
+      <c r="A5" s="29"/>
       <c r="B5" s="5"/>
       <c r="C5" s="8">
         <v>3</v>
@@ -1471,7 +1474,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="68">
-      <c r="A6" s="30"/>
+      <c r="A6" s="29"/>
       <c r="B6" s="5"/>
       <c r="C6" s="8">
         <v>4</v>
@@ -1491,7 +1494,7 @@
       <c r="H6" s="14"/>
     </row>
     <row r="7" spans="1:8" ht="68">
-      <c r="A7" s="30"/>
+      <c r="A7" s="29"/>
       <c r="B7" s="5"/>
       <c r="C7" s="8">
         <v>5</v>
@@ -1513,7 +1516,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="68">
-      <c r="A8" s="30"/>
+      <c r="A8" s="29"/>
       <c r="B8" s="5"/>
       <c r="C8" s="8">
         <v>6</v>
@@ -1535,7 +1538,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="68">
-      <c r="A9" s="30"/>
+      <c r="A9" s="29"/>
       <c r="B9" s="5"/>
       <c r="C9" s="8">
         <v>7</v>
@@ -1557,7 +1560,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="68">
-      <c r="A10" s="30"/>
+      <c r="A10" s="29"/>
       <c r="B10" s="5"/>
       <c r="C10" s="8">
         <v>8</v>
@@ -1589,7 +1592,7 @@
       <c r="H11" s="11"/>
     </row>
     <row r="12" spans="1:8" ht="35" thickTop="1">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="28" t="s">
         <v>186</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1613,7 +1616,7 @@
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" ht="51">
-      <c r="A13" s="30"/>
+      <c r="A13" s="29"/>
       <c r="B13" s="6"/>
       <c r="C13" s="18">
         <v>2</v>
@@ -1643,7 +1646,7 @@
       <c r="H14" s="11"/>
     </row>
     <row r="15" spans="1:8" ht="35" thickTop="1">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="28" t="s">
         <v>187</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -1667,7 +1670,7 @@
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" ht="34">
-      <c r="A16" s="30"/>
+      <c r="A16" s="29"/>
       <c r="B16" s="1"/>
       <c r="C16" s="18">
         <v>2</v>
@@ -1699,7 +1702,7 @@
       <c r="H17" s="11"/>
     </row>
     <row r="18" spans="1:11" ht="35" thickTop="1">
-      <c r="A18" s="32" t="s">
+      <c r="A18" s="28" t="s">
         <v>188</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1726,7 +1729,7 @@
       <c r="K18" s="19"/>
     </row>
     <row r="19" spans="1:11" ht="34">
-      <c r="A19" s="30"/>
+      <c r="A19" s="29"/>
       <c r="B19" s="1"/>
       <c r="C19" s="18">
         <v>2</v>
@@ -1759,7 +1762,7 @@
       <c r="H20" s="11"/>
     </row>
     <row r="21" spans="1:11" ht="52" thickTop="1">
-      <c r="A21" s="29" t="s">
+      <c r="A21" s="30" t="s">
         <v>189</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1783,7 +1786,7 @@
       <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:11" ht="17">
-      <c r="A22" s="30"/>
+      <c r="A22" s="29"/>
       <c r="C22" s="18">
         <v>2</v>
       </c>
@@ -1802,7 +1805,7 @@
       <c r="H22" s="1"/>
     </row>
     <row r="23" spans="1:11" ht="17">
-      <c r="A23" s="30"/>
+      <c r="A23" s="29"/>
       <c r="B23" s="1"/>
       <c r="C23" s="18">
         <v>3</v>
@@ -1822,7 +1825,7 @@
       <c r="H23" s="1"/>
     </row>
     <row r="24" spans="1:11" ht="17">
-      <c r="A24" s="30"/>
+      <c r="A24" s="29"/>
       <c r="B24" s="1"/>
       <c r="C24" s="18">
         <v>4</v>
@@ -1842,7 +1845,7 @@
       <c r="H24" s="1"/>
     </row>
     <row r="25" spans="1:11" ht="51">
-      <c r="A25" s="30"/>
+      <c r="A25" s="29"/>
       <c r="B25" s="1"/>
       <c r="C25" s="18">
         <v>5</v>
@@ -1862,7 +1865,7 @@
       <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:11" ht="34">
-      <c r="A26" s="30"/>
+      <c r="A26" s="29"/>
       <c r="B26" s="1"/>
       <c r="C26" s="18">
         <v>6</v>
@@ -1894,7 +1897,7 @@
       <c r="H27" s="11"/>
     </row>
     <row r="28" spans="1:11" ht="52" thickTop="1">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="30" t="s">
         <v>190</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -1918,7 +1921,7 @@
       <c r="H28" s="1"/>
     </row>
     <row r="29" spans="1:11" ht="17">
-      <c r="A29" s="30"/>
+      <c r="A29" s="29"/>
       <c r="B29" s="1"/>
       <c r="C29" s="18">
         <v>2</v>
@@ -1938,7 +1941,7 @@
       <c r="H29" s="1"/>
     </row>
     <row r="30" spans="1:11" ht="17">
-      <c r="A30" s="30"/>
+      <c r="A30" s="29"/>
       <c r="B30" s="1"/>
       <c r="C30" s="18">
         <v>3</v>
@@ -1958,7 +1961,7 @@
       <c r="H30" s="1"/>
     </row>
     <row r="31" spans="1:11" ht="51">
-      <c r="A31" s="30"/>
+      <c r="A31" s="29"/>
       <c r="B31" s="1"/>
       <c r="C31" s="18">
         <v>4</v>
@@ -1978,7 +1981,7 @@
       <c r="H31" s="1"/>
     </row>
     <row r="32" spans="1:11" ht="34">
-      <c r="A32" s="30"/>
+      <c r="A32" s="29"/>
       <c r="B32" s="1"/>
       <c r="C32" s="18">
         <v>5</v>
@@ -2010,7 +2013,7 @@
       <c r="H33" s="11"/>
     </row>
     <row r="34" spans="1:8" ht="52" thickTop="1">
-      <c r="A34" s="29" t="s">
+      <c r="A34" s="30" t="s">
         <v>191</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -2034,7 +2037,7 @@
       <c r="H34" s="1"/>
     </row>
     <row r="35" spans="1:8" ht="17">
-      <c r="A35" s="30"/>
+      <c r="A35" s="29"/>
       <c r="B35" s="1"/>
       <c r="C35" s="18">
         <v>2</v>
@@ -2054,7 +2057,7 @@
       <c r="H35" s="1"/>
     </row>
     <row r="36" spans="1:8" ht="17">
-      <c r="A36" s="30"/>
+      <c r="A36" s="29"/>
       <c r="B36" s="1"/>
       <c r="C36" s="18">
         <v>3</v>
@@ -2074,7 +2077,7 @@
       <c r="H36" s="1"/>
     </row>
     <row r="37" spans="1:8" ht="51">
-      <c r="A37" s="30"/>
+      <c r="A37" s="29"/>
       <c r="B37" s="1"/>
       <c r="C37" s="18">
         <v>4</v>
@@ -2094,7 +2097,7 @@
       <c r="H37" s="1"/>
     </row>
     <row r="38" spans="1:8" ht="34">
-      <c r="A38" s="30"/>
+      <c r="A38" s="29"/>
       <c r="B38" s="1"/>
       <c r="C38" s="18">
         <v>5</v>
@@ -2126,7 +2129,7 @@
       <c r="H39" s="11"/>
     </row>
     <row r="40" spans="1:8" ht="52" thickTop="1">
-      <c r="A40" s="29" t="s">
+      <c r="A40" s="30" t="s">
         <v>192</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -2152,7 +2155,7 @@
       </c>
     </row>
     <row r="41" spans="1:8" ht="34">
-      <c r="A41" s="30"/>
+      <c r="A41" s="29"/>
       <c r="B41" s="1"/>
       <c r="C41" s="20">
         <v>2</v>
@@ -2172,7 +2175,7 @@
       <c r="H41" s="1"/>
     </row>
     <row r="42" spans="1:8" ht="34">
-      <c r="A42" s="30"/>
+      <c r="A42" s="29"/>
       <c r="B42" s="1"/>
       <c r="C42" s="20">
         <v>3</v>
@@ -2192,7 +2195,7 @@
       <c r="H42" s="1"/>
     </row>
     <row r="43" spans="1:8" ht="34">
-      <c r="A43" s="30"/>
+      <c r="A43" s="29"/>
       <c r="B43" s="1"/>
       <c r="C43" s="20">
         <v>4</v>
@@ -2212,7 +2215,7 @@
       <c r="H43" s="1"/>
     </row>
     <row r="44" spans="1:8" ht="34">
-      <c r="A44" s="30"/>
+      <c r="A44" s="29"/>
       <c r="B44" s="1"/>
       <c r="C44" s="20">
         <v>5</v>
@@ -2242,7 +2245,7 @@
       <c r="H45" s="11"/>
     </row>
     <row r="46" spans="1:8" ht="52" thickTop="1">
-      <c r="A46" s="27" t="s">
+      <c r="A46" s="31" t="s">
         <v>193</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -2266,7 +2269,7 @@
       <c r="H46" s="1"/>
     </row>
     <row r="47" spans="1:8" ht="51">
-      <c r="A47" s="28"/>
+      <c r="A47" s="32"/>
       <c r="B47" s="6"/>
       <c r="C47" s="18">
         <v>2</v>
@@ -2286,7 +2289,7 @@
       <c r="H47" s="1"/>
     </row>
     <row r="48" spans="1:8" ht="34">
-      <c r="A48" s="28"/>
+      <c r="A48" s="32"/>
       <c r="B48" s="6"/>
       <c r="C48" s="18">
         <v>3</v>
@@ -2306,7 +2309,7 @@
       <c r="H48" s="1"/>
     </row>
     <row r="49" spans="1:8" ht="34">
-      <c r="A49" s="28"/>
+      <c r="A49" s="32"/>
       <c r="B49" s="6"/>
       <c r="C49" s="18">
         <v>4</v>
@@ -2326,7 +2329,7 @@
       <c r="H49" s="1"/>
     </row>
     <row r="50" spans="1:8" ht="34">
-      <c r="A50" s="28"/>
+      <c r="A50" s="32"/>
       <c r="B50" s="6"/>
       <c r="C50" s="18">
         <v>5</v>
@@ -2346,7 +2349,7 @@
       <c r="H50" s="1"/>
     </row>
     <row r="51" spans="1:8" ht="34">
-      <c r="A51" s="28"/>
+      <c r="A51" s="32"/>
       <c r="B51" s="6"/>
       <c r="C51" s="18">
         <v>6</v>
@@ -2366,7 +2369,7 @@
       <c r="H51" s="1"/>
     </row>
     <row r="52" spans="1:8" ht="34">
-      <c r="A52" s="28"/>
+      <c r="A52" s="32"/>
       <c r="B52" s="6"/>
       <c r="C52" s="18">
         <v>7</v>
@@ -2396,7 +2399,7 @@
       <c r="H53" s="11"/>
     </row>
     <row r="54" spans="1:8" ht="35" customHeight="1" thickTop="1">
-      <c r="A54" s="27" t="s">
+      <c r="A54" s="31" t="s">
         <v>194</v>
       </c>
       <c r="B54" s="1" t="s">
@@ -2420,7 +2423,7 @@
       <c r="H54" s="1"/>
     </row>
     <row r="55" spans="1:8" ht="34">
-      <c r="A55" s="28"/>
+      <c r="A55" s="32"/>
       <c r="B55" s="6"/>
       <c r="C55" s="18">
         <v>2</v>
@@ -2440,7 +2443,7 @@
       <c r="H55" s="1"/>
     </row>
     <row r="56" spans="1:8" ht="34">
-      <c r="A56" s="28"/>
+      <c r="A56" s="32"/>
       <c r="B56" s="6"/>
       <c r="C56" s="18">
         <v>3</v>
@@ -2460,7 +2463,7 @@
       <c r="H56" s="1"/>
     </row>
     <row r="57" spans="1:8" ht="34">
-      <c r="A57" s="28"/>
+      <c r="A57" s="32"/>
       <c r="B57" s="6"/>
       <c r="C57" s="18">
         <v>4</v>
@@ -2480,7 +2483,7 @@
       <c r="H57" s="1"/>
     </row>
     <row r="58" spans="1:8" ht="51">
-      <c r="A58" s="28"/>
+      <c r="A58" s="32"/>
       <c r="B58" s="6"/>
       <c r="C58" s="18">
         <v>5</v>
@@ -2500,7 +2503,7 @@
       <c r="H58" s="1"/>
     </row>
     <row r="59" spans="1:8" ht="34">
-      <c r="A59" s="28"/>
+      <c r="A59" s="32"/>
       <c r="B59" s="6"/>
       <c r="C59" s="18">
         <v>6</v>
@@ -2520,7 +2523,7 @@
       <c r="H59" s="1"/>
     </row>
     <row r="60" spans="1:8" ht="34">
-      <c r="A60" s="28"/>
+      <c r="A60" s="32"/>
       <c r="B60" s="6"/>
       <c r="C60" s="18">
         <v>7</v>
@@ -2550,7 +2553,7 @@
       <c r="H61" s="11"/>
     </row>
     <row r="62" spans="1:8" ht="35" thickTop="1">
-      <c r="A62" s="27" t="s">
+      <c r="A62" s="31" t="s">
         <v>195</v>
       </c>
       <c r="B62" s="1" t="s">
@@ -2574,7 +2577,7 @@
       <c r="H62" s="1"/>
     </row>
     <row r="63" spans="1:8" ht="85">
-      <c r="A63" s="28"/>
+      <c r="A63" s="32"/>
       <c r="B63" s="6"/>
       <c r="C63" s="18">
         <v>2</v>
@@ -2594,7 +2597,7 @@
       <c r="H63" s="1"/>
     </row>
     <row r="64" spans="1:8" ht="85">
-      <c r="A64" s="28"/>
+      <c r="A64" s="32"/>
       <c r="B64" s="6"/>
       <c r="C64" s="18">
         <v>3</v>
@@ -2626,7 +2629,7 @@
       <c r="H65" s="11"/>
     </row>
     <row r="66" spans="1:8" ht="52" thickTop="1">
-      <c r="A66" s="27" t="s">
+      <c r="A66" s="31" t="s">
         <v>196</v>
       </c>
       <c r="B66" s="1" t="s">
@@ -2650,7 +2653,7 @@
       <c r="H66" s="1"/>
     </row>
     <row r="67" spans="1:8" ht="17">
-      <c r="A67" s="28"/>
+      <c r="A67" s="32"/>
       <c r="B67" s="6"/>
       <c r="C67" s="18">
         <v>2</v>
@@ -2670,7 +2673,7 @@
       <c r="H67" s="1"/>
     </row>
     <row r="68" spans="1:8" ht="34">
-      <c r="A68" s="28"/>
+      <c r="A68" s="32"/>
       <c r="B68" s="18"/>
       <c r="C68" s="18">
         <v>3</v>
@@ -2700,7 +2703,7 @@
       <c r="H69" s="11"/>
     </row>
     <row r="70" spans="1:8" ht="52" thickTop="1">
-      <c r="A70" s="27" t="s">
+      <c r="A70" s="31" t="s">
         <v>197</v>
       </c>
       <c r="B70" s="1" t="s">
@@ -2724,7 +2727,7 @@
       <c r="H70" s="1"/>
     </row>
     <row r="71" spans="1:8" ht="34">
-      <c r="A71" s="28"/>
+      <c r="A71" s="32"/>
       <c r="B71" s="1"/>
       <c r="C71" s="18">
         <v>2</v>
@@ -2744,7 +2747,7 @@
       <c r="H71" s="1"/>
     </row>
     <row r="72" spans="1:8" ht="34">
-      <c r="A72" s="28"/>
+      <c r="A72" s="32"/>
       <c r="B72" s="1"/>
       <c r="C72" s="18">
         <v>3</v>
@@ -2764,7 +2767,7 @@
       <c r="H72" s="1"/>
     </row>
     <row r="73" spans="1:8" ht="34">
-      <c r="A73" s="28"/>
+      <c r="A73" s="32"/>
       <c r="B73" s="1"/>
       <c r="C73" s="18">
         <v>4</v>
@@ -2784,7 +2787,7 @@
       <c r="H73" s="1"/>
     </row>
     <row r="74" spans="1:8" ht="34">
-      <c r="A74" s="28"/>
+      <c r="A74" s="32"/>
       <c r="B74" s="1"/>
       <c r="C74" s="18">
         <v>5</v>
@@ -2804,7 +2807,7 @@
       <c r="H74" s="1"/>
     </row>
     <row r="75" spans="1:8" ht="17">
-      <c r="A75" s="28"/>
+      <c r="A75" s="32"/>
       <c r="B75" s="1"/>
       <c r="C75" s="18">
         <v>6</v>
@@ -2834,7 +2837,7 @@
       <c r="H76" s="11"/>
     </row>
     <row r="77" spans="1:8" ht="52" thickTop="1">
-      <c r="A77" s="27" t="s">
+      <c r="A77" s="31" t="s">
         <v>198</v>
       </c>
       <c r="B77" s="1" t="s">
@@ -2858,7 +2861,7 @@
       <c r="H77" s="1"/>
     </row>
     <row r="78" spans="1:8" ht="34">
-      <c r="A78" s="28"/>
+      <c r="A78" s="32"/>
       <c r="B78" s="1"/>
       <c r="C78" s="18">
         <v>2</v>
@@ -2878,7 +2881,7 @@
       <c r="H78" s="1"/>
     </row>
     <row r="79" spans="1:8" ht="51">
-      <c r="A79" s="28"/>
+      <c r="A79" s="32"/>
       <c r="B79" s="1"/>
       <c r="C79" s="18">
         <v>3</v>
@@ -2900,7 +2903,7 @@
       </c>
     </row>
     <row r="80" spans="1:8" ht="34">
-      <c r="A80" s="28"/>
+      <c r="A80" s="32"/>
       <c r="B80" s="1"/>
       <c r="C80" s="18">
         <v>4</v>
@@ -2920,7 +2923,7 @@
       <c r="H80" s="1"/>
     </row>
     <row r="81" spans="1:8" ht="17">
-      <c r="A81" s="28"/>
+      <c r="A81" s="32"/>
       <c r="B81" s="1"/>
       <c r="C81" s="18">
         <v>5</v>
@@ -2950,7 +2953,7 @@
       <c r="H82" s="11"/>
     </row>
     <row r="83" spans="1:8" ht="52" thickTop="1">
-      <c r="A83" s="27" t="s">
+      <c r="A83" s="31" t="s">
         <v>199</v>
       </c>
       <c r="B83" s="1" t="s">
@@ -2974,7 +2977,7 @@
       <c r="H83" s="1"/>
     </row>
     <row r="84" spans="1:8" ht="34">
-      <c r="A84" s="28"/>
+      <c r="A84" s="32"/>
       <c r="B84" s="1"/>
       <c r="C84" s="18">
         <v>2</v>
@@ -2994,7 +2997,7 @@
       <c r="H84" s="1"/>
     </row>
     <row r="85" spans="1:8" ht="34">
-      <c r="A85" s="28"/>
+      <c r="A85" s="32"/>
       <c r="B85" s="1"/>
       <c r="C85" s="18">
         <v>3</v>
@@ -3014,7 +3017,7 @@
       <c r="H85" s="1"/>
     </row>
     <row r="86" spans="1:8" ht="51">
-      <c r="A86" s="28"/>
+      <c r="A86" s="32"/>
       <c r="B86" s="1"/>
       <c r="C86" s="18">
         <v>4</v>
@@ -3046,7 +3049,7 @@
       <c r="H87" s="11"/>
     </row>
     <row r="88" spans="1:8" ht="52" thickTop="1">
-      <c r="A88" s="27" t="s">
+      <c r="A88" s="31" t="s">
         <v>200</v>
       </c>
       <c r="B88" s="1" t="s">
@@ -3070,7 +3073,7 @@
       <c r="H88" s="1"/>
     </row>
     <row r="89" spans="1:8" ht="34">
-      <c r="A89" s="28"/>
+      <c r="A89" s="32"/>
       <c r="B89" s="1"/>
       <c r="C89" s="18">
         <v>2</v>
@@ -3090,7 +3093,7 @@
       <c r="H89" s="1"/>
     </row>
     <row r="90" spans="1:8" ht="17">
-      <c r="A90" s="28"/>
+      <c r="A90" s="32"/>
       <c r="B90" s="1"/>
       <c r="C90" s="18">
         <v>3</v>
@@ -3110,7 +3113,7 @@
       <c r="H90" s="1"/>
     </row>
     <row r="91" spans="1:8" ht="68">
-      <c r="A91" s="28"/>
+      <c r="A91" s="32"/>
       <c r="B91" s="1"/>
       <c r="C91" s="18">
         <v>4</v>
@@ -3130,7 +3133,7 @@
       <c r="H91" s="1"/>
     </row>
     <row r="92" spans="1:8" ht="34">
-      <c r="A92" s="28"/>
+      <c r="A92" s="32"/>
       <c r="B92" s="1"/>
       <c r="C92" s="18">
         <v>5</v>
@@ -3160,7 +3163,7 @@
       <c r="H93" s="11"/>
     </row>
     <row r="94" spans="1:8" ht="33" customHeight="1" thickTop="1">
-      <c r="A94" s="27" t="s">
+      <c r="A94" s="31" t="s">
         <v>201</v>
       </c>
       <c r="B94" s="21" t="s">
@@ -3184,7 +3187,7 @@
       <c r="H94" s="21"/>
     </row>
     <row r="95" spans="1:8" ht="32">
-      <c r="A95" s="28"/>
+      <c r="A95" s="32"/>
       <c r="B95" s="24"/>
       <c r="C95" s="25">
         <v>2</v>
@@ -3204,7 +3207,7 @@
       <c r="H95" s="24"/>
     </row>
     <row r="96" spans="1:8" ht="32">
-      <c r="A96" s="28"/>
+      <c r="A96" s="32"/>
       <c r="B96" s="24"/>
       <c r="C96" s="25">
         <v>3</v>
@@ -3224,7 +3227,7 @@
       <c r="H96" s="24"/>
     </row>
     <row r="97" spans="1:8">
-      <c r="A97" s="28"/>
+      <c r="A97" s="32"/>
       <c r="B97" s="24"/>
       <c r="C97" s="25">
         <v>4</v>
@@ -3246,7 +3249,7 @@
       </c>
     </row>
     <row r="98" spans="1:8">
-      <c r="A98" s="28"/>
+      <c r="A98" s="32"/>
       <c r="B98" s="24"/>
       <c r="C98" s="25">
         <v>5</v>
@@ -3266,7 +3269,7 @@
       <c r="H98" s="24"/>
     </row>
     <row r="99" spans="1:8" ht="32">
-      <c r="A99" s="28"/>
+      <c r="A99" s="32"/>
       <c r="B99" s="24"/>
       <c r="C99" s="25">
         <v>6</v>
@@ -3286,7 +3289,7 @@
       <c r="H99" s="24"/>
     </row>
     <row r="100" spans="1:8" ht="32">
-      <c r="A100" s="28"/>
+      <c r="A100" s="32"/>
       <c r="B100" s="24"/>
       <c r="C100" s="25">
         <v>7</v>
@@ -3306,7 +3309,7 @@
       <c r="H100" s="24"/>
     </row>
     <row r="101" spans="1:8" ht="32">
-      <c r="A101" s="28"/>
+      <c r="A101" s="32"/>
       <c r="B101" s="24"/>
       <c r="C101" s="25">
         <v>8</v>
@@ -3326,7 +3329,7 @@
       <c r="H101" s="24"/>
     </row>
     <row r="102" spans="1:8" ht="32">
-      <c r="A102" s="28"/>
+      <c r="A102" s="32"/>
       <c r="B102" s="24"/>
       <c r="C102" s="25">
         <v>9</v>
@@ -3356,7 +3359,7 @@
       <c r="H103" s="11"/>
     </row>
     <row r="104" spans="1:8" ht="55" customHeight="1" thickTop="1">
-      <c r="A104" s="27" t="s">
+      <c r="A104" s="31" t="s">
         <v>202</v>
       </c>
       <c r="B104" s="21" t="s">
@@ -3380,7 +3383,7 @@
       <c r="H104" s="21"/>
     </row>
     <row r="105" spans="1:8" ht="32">
-      <c r="A105" s="28"/>
+      <c r="A105" s="32"/>
       <c r="B105" s="24"/>
       <c r="C105" s="25">
         <v>2</v>
@@ -3400,7 +3403,7 @@
       <c r="H105" s="24"/>
     </row>
     <row r="106" spans="1:8" ht="32">
-      <c r="A106" s="28"/>
+      <c r="A106" s="32"/>
       <c r="B106" s="24"/>
       <c r="C106" s="25">
         <v>3</v>
@@ -3419,8 +3422,8 @@
       </c>
       <c r="H106" s="24"/>
     </row>
-    <row r="107" spans="1:8">
-      <c r="A107" s="28"/>
+    <row r="107" spans="1:8" ht="17">
+      <c r="A107" s="32"/>
       <c r="B107" s="24"/>
       <c r="C107" s="25">
         <v>4</v>
@@ -3437,10 +3440,12 @@
       <c r="G107" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="H107" s="24"/>
+      <c r="H107" s="1" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="108" spans="1:8">
-      <c r="A108" s="28"/>
+      <c r="A108" s="32"/>
       <c r="B108" s="24"/>
       <c r="C108" s="25">
         <v>5</v>
@@ -3460,7 +3465,7 @@
       <c r="H108" s="24"/>
     </row>
     <row r="109" spans="1:8" ht="32">
-      <c r="A109" s="28"/>
+      <c r="A109" s="32"/>
       <c r="B109" s="24"/>
       <c r="C109" s="25">
         <v>6</v>
@@ -3480,7 +3485,7 @@
       <c r="H109" s="24"/>
     </row>
     <row r="110" spans="1:8" ht="32">
-      <c r="A110" s="28"/>
+      <c r="A110" s="32"/>
       <c r="B110" s="24"/>
       <c r="C110" s="25">
         <v>7</v>
@@ -3500,7 +3505,7 @@
       <c r="H110" s="24"/>
     </row>
     <row r="111" spans="1:8" ht="32">
-      <c r="A111" s="28"/>
+      <c r="A111" s="32"/>
       <c r="B111" s="24"/>
       <c r="C111" s="25">
         <v>8</v>
@@ -3520,7 +3525,7 @@
       <c r="H111" s="24"/>
     </row>
     <row r="112" spans="1:8" ht="32">
-      <c r="A112" s="28"/>
+      <c r="A112" s="32"/>
       <c r="B112" s="24"/>
       <c r="C112" s="25">
         <v>9</v>
@@ -3550,7 +3555,7 @@
       <c r="H113" s="11"/>
     </row>
     <row r="114" spans="1:8" ht="52" thickTop="1">
-      <c r="A114" s="27" t="s">
+      <c r="A114" s="31" t="s">
         <v>203</v>
       </c>
       <c r="B114" s="1" t="s">
@@ -3576,7 +3581,7 @@
       </c>
     </row>
     <row r="115" spans="1:8" ht="17">
-      <c r="A115" s="28"/>
+      <c r="A115" s="32"/>
       <c r="B115" s="1"/>
       <c r="C115" s="18">
         <v>2</v>
@@ -3606,7 +3611,7 @@
       <c r="H116" s="11"/>
     </row>
     <row r="117" spans="1:8" ht="52" thickTop="1">
-      <c r="A117" s="27" t="s">
+      <c r="A117" s="31" t="s">
         <v>204</v>
       </c>
       <c r="B117" s="1" t="s">
@@ -3630,7 +3635,7 @@
       <c r="H117" s="1"/>
     </row>
     <row r="118" spans="1:8" ht="17">
-      <c r="A118" s="28"/>
+      <c r="A118" s="32"/>
       <c r="B118" s="6"/>
       <c r="C118" s="18">
         <v>2</v>
@@ -3660,7 +3665,7 @@
       <c r="H119" s="11"/>
     </row>
     <row r="120" spans="1:8" ht="35" thickTop="1">
-      <c r="A120" s="27" t="s">
+      <c r="A120" s="31" t="s">
         <v>205</v>
       </c>
       <c r="B120" s="1" t="s">
@@ -3684,7 +3689,7 @@
       <c r="H120" s="1"/>
     </row>
     <row r="121" spans="1:8" ht="17">
-      <c r="A121" s="28"/>
+      <c r="A121" s="32"/>
       <c r="B121" s="1"/>
       <c r="C121" s="18">
         <v>2</v>
@@ -3716,16 +3721,11 @@
     <row r="123" spans="1:8" ht="17" thickTop="1"/>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A3:A10"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A34:A38"/>
-    <mergeCell ref="A40:A44"/>
-    <mergeCell ref="A46:A52"/>
-    <mergeCell ref="A21:A26"/>
-    <mergeCell ref="A28:A32"/>
+    <mergeCell ref="A120:A121"/>
+    <mergeCell ref="A94:A102"/>
+    <mergeCell ref="A104:A112"/>
+    <mergeCell ref="A114:A115"/>
+    <mergeCell ref="A117:A118"/>
     <mergeCell ref="A77:A81"/>
     <mergeCell ref="A83:A86"/>
     <mergeCell ref="A88:A92"/>
@@ -3733,11 +3733,16 @@
     <mergeCell ref="A62:A64"/>
     <mergeCell ref="A66:A68"/>
     <mergeCell ref="A70:A75"/>
-    <mergeCell ref="A120:A121"/>
-    <mergeCell ref="A94:A102"/>
-    <mergeCell ref="A104:A112"/>
-    <mergeCell ref="A114:A115"/>
-    <mergeCell ref="A117:A118"/>
+    <mergeCell ref="A34:A38"/>
+    <mergeCell ref="A40:A44"/>
+    <mergeCell ref="A46:A52"/>
+    <mergeCell ref="A21:A26"/>
+    <mergeCell ref="A28:A32"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A3:A10"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A18:A19"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D15" r:id="rId1" display="https://jshint.com/" xr:uid="{2763C512-0362-9F4A-B6E9-4326ACCC5667}"/>

</xml_diff>